<commit_message>
results with zero temperature
</commit_message>
<xml_diff>
--- a/results/classification_results.xlsx
+++ b/results/classification_results.xlsx
@@ -508,7 +508,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
+          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
         </is>
       </c>
       <c r="D4" t="b">
@@ -768,7 +768,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
+          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
         </is>
       </c>
       <c r="D17" t="b">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="D21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -928,7 +928,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
+          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
         </is>
       </c>
       <c r="D25" t="b">
@@ -1108,11 +1108,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GEOGRAPHY_QA</t>
         </is>
       </c>
       <c r="D34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1348,11 +1348,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GEOGRAPHY_QA</t>
         </is>
       </c>
       <c r="D46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>IMAGE_SEGMENTATION</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D47" t="b">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
         </is>
       </c>
       <c r="D48" t="b">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>IMAGE_SEGMENTATION</t>
+          <t>OBJECT_COUNTING</t>
         </is>
       </c>
       <c r="D49" t="b">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
         </is>
       </c>
       <c r="D51" t="b">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D53" t="b">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>IMAGE_SEGMENTATION</t>
+          <t>OBJECT_COUNTING</t>
         </is>
       </c>
       <c r="D54" t="b">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>IMAGE_SEGMENTATION</t>
+          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
         </is>
       </c>
       <c r="D56" t="b">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>IMAGE_SEGMENTATION</t>
         </is>
       </c>
       <c r="D58" t="b">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>OBJECT_COUNTING</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D59" t="b">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>OBJECT_COUNTING</t>
+          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
         </is>
       </c>
       <c r="D60" t="b">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>OBJECT_COUNTING</t>
         </is>
       </c>
       <c r="D61" t="b">

</xml_diff>

<commit_message>
binary visual QA explanation
</commit_message>
<xml_diff>
--- a/results/classification_results.xlsx
+++ b/results/classification_results.xlsx
@@ -1068,7 +1068,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D32" t="b">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D33" t="b">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D34" t="b">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D35" t="b">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D36" t="b">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D37" t="b">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D38" t="b">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D39" t="b">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D40" t="b">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D41" t="b">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D42" t="b">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D43" t="b">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D44" t="b">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D45" t="b">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>GEOGRAPHY_QA</t>
+          <t>GEOSPATIAL_QA</t>
         </is>
       </c>
       <c r="D46" t="b">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1383,12 +1383,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D48" t="b">
@@ -1403,12 +1403,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>OBJECT_COUNTING</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D49" t="b">
@@ -1423,12 +1423,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>IMAGE_SEGMENTATION</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D50" t="b">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1463,12 +1463,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>IMAGE_SEGMENTATION</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D52" t="b">
@@ -1483,12 +1483,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D53" t="b">
@@ -1503,12 +1503,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>OBJECT_COUNTING</t>
+          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
         </is>
       </c>
       <c r="D54" t="b">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1563,12 +1563,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>IMAGE_SEGMENTATION</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D57" t="b">
@@ -1583,12 +1583,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>IMAGE_SEGMENTATION</t>
+          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
         </is>
       </c>
       <c r="D58" t="b">
@@ -1603,12 +1603,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
         </is>
       </c>
       <c r="D59" t="b">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D60" t="b">
@@ -1643,12 +1643,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>VISUAL_QA</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>OBJECT_COUNTING</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D61" t="b">

</xml_diff>

<commit_message>
evaluation and hierarchy change
</commit_message>
<xml_diff>
--- a/results/classification_results.xlsx
+++ b/results/classification_results.xlsx
@@ -928,7 +928,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
+          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
         </is>
       </c>
       <c r="D25" t="b">
@@ -948,7 +948,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
+          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
         </is>
       </c>
       <c r="D26" t="b">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D47" t="b">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D51" t="b">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D54" t="b">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D55" t="b">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D56" t="b">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D58" t="b">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_IMAGE</t>
+          <t>BINARY_VISUAL_QA</t>
         </is>
       </c>
       <c r="D59" t="b">

</xml_diff>

<commit_message>
added main and made a slight difference in a prompt
</commit_message>
<xml_diff>
--- a/results/classification_results.xlsx
+++ b/results/classification_results.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
+          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
         </is>
       </c>
       <c r="D5" t="b">
@@ -568,7 +568,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
+          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
         </is>
       </c>
       <c r="D7" t="b">
@@ -668,11 +668,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
         </is>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -708,7 +708,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
+          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
         </is>
       </c>
       <c r="D14" t="b">
@@ -848,7 +848,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
         </is>
       </c>
       <c r="D21" t="b">
@@ -928,7 +928,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>IMAGE_RETRIEVAL_BY_CAPTION</t>
+          <t>IMAGE_RETRIEVAL_BY_METADATA</t>
         </is>
       </c>
       <c r="D25" t="b">

</xml_diff>